<commit_message>
Debug all scripts under regression test folder.
</commit_message>
<xml_diff>
--- a/NformTester/NformTester/Keywordscripts/400.10.20_ApplicationRestartSession.xlsx
+++ b/NformTester/NformTester/Keywordscripts/400.10.20_ApplicationRestartSession.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="270" yWindow="2535" windowWidth="18195" windowHeight="14070"/>
@@ -1200,7 +1200,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7101" uniqueCount="811">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7101" uniqueCount="809">
   <si>
     <t>FormLogin_to_LiebertR_Nform</t>
   </si>
@@ -3637,25 +3637,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>T</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ALARMSLiebertRNform</t>
-  </si>
-  <si>
-    <t>NAVIGATELiebertRNform</t>
-  </si>
-  <si>
-    <t>Buttonminnavigate</t>
-  </si>
-  <si>
-    <t>Buttonminalarm</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
     <t>C</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -3671,6 +3652,20 @@
   </si>
   <si>
     <t>Error</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALARMSNAVIGATELiebertRNform</t>
+  </si>
+  <si>
+    <t>Buttonmin</t>
+  </si>
+  <si>
+    <t>;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4628,8 +4623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O189"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -4639,7 +4634,7 @@
     <col min="5" max="5" width="27.75" customWidth="1"/>
     <col min="6" max="6" width="33" customWidth="1"/>
     <col min="7" max="7" width="18.875" customWidth="1"/>
-    <col min="8" max="8" width="17.875" customWidth="1"/>
+    <col min="8" max="8" width="21.625" customWidth="1"/>
     <col min="9" max="9" width="16.875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4759,7 +4754,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>800</v>
+        <v>807</v>
       </c>
       <c r="E4" s="14" t="s">
         <v>191</v>
@@ -4822,10 +4817,10 @@
         <v>786</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>802</v>
+        <v>805</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>803</v>
+        <v>806</v>
       </c>
       <c r="G6" s="19" t="s">
         <v>2</v>
@@ -4882,10 +4877,10 @@
         <v>786</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>801</v>
+        <v>805</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>804</v>
+        <v>806</v>
       </c>
       <c r="G8" s="19" t="s">
         <v>2</v>
@@ -4966,10 +4961,10 @@
         <v>10</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>806</v>
+        <v>800</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>807</v>
+        <v>801</v>
       </c>
       <c r="F11" s="20">
         <v>2</v>
@@ -4993,18 +4988,18 @@
         <v>11</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>805</v>
+        <v>808</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>808</v>
+        <v>802</v>
       </c>
       <c r="F12" s="20"/>
       <c r="G12" s="20"/>
       <c r="H12" s="19" t="s">
-        <v>809</v>
+        <v>803</v>
       </c>
       <c r="I12" s="19" t="s">
-        <v>810</v>
+        <v>804</v>
       </c>
       <c r="J12" s="20" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Add link in report, and add function to check whether Nform Server is stopped or not.
</commit_message>
<xml_diff>
--- a/NformTester/NformTester/Keywordscripts/400.10.20_ApplicationRestartSession.xlsx
+++ b/NformTester/NformTester/Keywordscripts/400.10.20_ApplicationRestartSession.xlsx
@@ -4623,8 +4623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>

</xml_diff>